<commit_message>
Added new commodity coase grain
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -9,6 +9,8 @@
     <sheet name="rice" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="wheat" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="rra" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="coarse grain" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="coarse_grain" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -461,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +496,191 @@
         <is>
           <t>Commodity</t>
         </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BXC</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BXC</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BHT</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DMSJ</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BHT</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BHT</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>DMSJ</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BHT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,13 +710,88 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>To</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NMH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>JPTN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Andhra Pradesh</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>KSA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>FCIG</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Andhra Pradesh</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,30 +821,220 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>To</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BGBR</t>
+          <t>BHT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VSG</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>RRA</t>
         </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RJY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Coarse Grain</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RJY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Coarse Grain</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added three commmodites i.e w+frk, frk rra, frk br
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -11,6 +11,9 @@
     <sheet name="rra" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="coarse grain" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="coarse_grain" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="frk_rra" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="frk_br" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="frk" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -694,7 +697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,66 +735,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>NMH</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MP</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>JPTN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Andhra Pradesh</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>KSA</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Punjab</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>FCIG</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Andhra Pradesh</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -805,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,36 +786,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BHT</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NNA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Bihar</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RRA</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +880,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,34 +920,157 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>RJY</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CTO</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Bihar</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Coarse Grain</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added last commodity and added validation in frontend
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -14,6 +14,8 @@
     <sheet name="frk_rra" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="frk_br" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="frk" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="frkcgr" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="wcgr" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -691,7 +693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -742,13 +744,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,6 +788,117 @@
         <is>
           <t>Values</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BAT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BMKI</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>JAT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jammu &amp; Kashmir</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>VSG</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>RRA</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1076,4 +1189,55 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>From State</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>To State</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
done checks for other commodites
</commit_message>
<xml_diff>
--- a/Output/List_DPT.xlsx
+++ b/Output/List_DPT.xlsx
@@ -750,7 +750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,30 +793,150 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BAT</t>
+          <t>FCSM</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DMSJ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FCSM</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>KSNG</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BGTN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Punjab</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>BMKI</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BBU</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Bihar</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Wheat</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KSA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NNA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>JNL</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>KSNG</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -831,7 +951,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,36 +989,6 @@
         <is>
           <t>Values</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>JAT</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jammu &amp; Kashmir</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>VSG</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Goa</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>RRA</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>